<commit_message>
Some updates on file templating
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -22,14 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>de</t>
   </si>
   <si>
-    <t>Mo-Fr: 07:00-17:00; Sa: 07:00-12:00</t>
-  </si>
-  <si>
     <t>Ja</t>
   </si>
   <si>
@@ -117,24 +114,9 @@
     <t>Schwarzs GmbH</t>
   </si>
   <si>
-    <t>lkw-schwarz@t-online.de</t>
-  </si>
-  <si>
     <t>Losheim am See</t>
   </si>
   <si>
-    <t>Michaela Schwarz</t>
-  </si>
-  <si>
-    <t>0049 6872 90110</t>
-  </si>
-  <si>
-    <t>0049 6872 901117</t>
-  </si>
-  <si>
-    <t>Freie Werkstatts</t>
-  </si>
-  <si>
     <t>pid</t>
   </si>
   <si>
@@ -145,13 +127,31 @@
   </si>
   <si>
     <t>+496872901117</t>
+  </si>
+  <si>
+    <t>example@email.com</t>
+  </si>
+  <si>
+    <t>Michael Carmichael</t>
+  </si>
+  <si>
+    <t>09289829</t>
+  </si>
+  <si>
+    <t>example@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy </t>
+  </si>
+  <si>
+    <t>dummy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +187,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -248,12 +256,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2"/>
@@ -261,10 +270,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
     <cellStyle name="Besuchter Link" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -535,7 +546,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -545,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -583,88 +594,88 @@
   <sheetData>
     <row r="1" spans="1:30" ht="15">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
@@ -677,46 +688,46 @@
         <v>858120</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="4">
         <v>66679</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2">
+        <v>9898</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="P2" t="s">
         <v>40</v>
-      </c>
-      <c r="J2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" t="s">
-        <v>1</v>
       </c>
       <c r="Q2" s="4">
         <v>6.7605300000000002</v>
@@ -725,34 +736,34 @@
         <v>49.511389999999999</v>
       </c>
       <c r="S2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="15">
@@ -769,8 +780,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="email@email.com"/>
-    <hyperlink ref="N2" r:id="rId2" display="wh@email.com"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="N2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
added some documentation and code note
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="3540" windowWidth="26400" windowHeight="11340"/>
+    <workbookView xWindow="4100" yWindow="3320" windowWidth="26400" windowHeight="11340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>de</t>
   </si>
   <si>
-    <t>Ja</t>
-  </si>
-  <si>
     <t xml:space="preserve">workshopid </t>
   </si>
   <si>
@@ -66,48 +63,6 @@
     <t>email_warehouse</t>
   </si>
   <si>
-    <t>partner_of</t>
-  </si>
-  <si>
-    <t>business hours</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">latitude </t>
-  </si>
-  <si>
-    <t>braketest</t>
-  </si>
-  <si>
-    <t>diagnose</t>
-  </si>
-  <si>
-    <t>service_brakes</t>
-  </si>
-  <si>
-    <t>service hydraulics</t>
-  </si>
-  <si>
-    <t>service_tyres</t>
-  </si>
-  <si>
-    <t>service_chiller</t>
-  </si>
-  <si>
-    <t>service_crane</t>
-  </si>
-  <si>
-    <t>service_liftgate</t>
-  </si>
-  <si>
-    <t>service_construction</t>
-  </si>
-  <si>
-    <t>service_anhaenger</t>
-  </si>
-  <si>
     <t>Hauptstr.  155</t>
   </si>
   <si>
@@ -139,12 +94,6 @@
   </si>
   <si>
     <t>example@example.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dummy </t>
-  </si>
-  <si>
-    <t>dummy</t>
   </si>
 </sst>
 </file>
@@ -262,9 +211,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -546,7 +494,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -554,133 +502,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="7" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="20.5" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="19.5" style="4" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="14" style="4" customWidth="1"/>
-    <col min="16" max="16" width="24.83203125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.5" style="4" customWidth="1"/>
-    <col min="18" max="18" width="13.83203125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" style="4" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="14.1640625" style="4" customWidth="1"/>
-    <col min="22" max="22" width="15.83203125" style="4" customWidth="1"/>
-    <col min="23" max="23" width="15" style="4" customWidth="1"/>
-    <col min="24" max="24" width="13.5" style="4" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" style="4" customWidth="1"/>
-    <col min="26" max="26" width="15.6640625" style="4" customWidth="1"/>
-    <col min="27" max="27" width="18.6640625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="16.5" style="4" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7" style="3" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="20.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="14" style="3" customWidth="1"/>
+    <col min="16" max="16" width="24.83203125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="14.5" style="3" customWidth="1"/>
+    <col min="18" max="18" width="13.83203125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="14.1640625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="15.83203125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="15" style="3" customWidth="1"/>
+    <col min="24" max="24" width="13.5" style="3" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" style="3" customWidth="1"/>
+    <col min="26" max="26" width="15.6640625" style="3" customWidth="1"/>
+    <col min="27" max="27" width="18.6640625" style="3" customWidth="1"/>
+    <col min="28" max="28" width="16.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15">
-      <c r="A1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:28" ht="15">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
+      <c r="W1"/>
+      <c r="X1"/>
+      <c r="Y1"/>
+      <c r="Z1"/>
+      <c r="AA1"/>
+      <c r="AB1"/>
     </row>
-    <row r="2" spans="1:30" ht="15">
+    <row r="2" spans="1:28">
       <c r="A2">
         <v>1</v>
       </c>
@@ -688,95 +606,67 @@
         <v>858120</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="4">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3">
         <v>66679</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>35</v>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="M2">
         <v>9898</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>6.7605300000000002</v>
-      </c>
-      <c r="R2" s="4">
-        <v>49.511389999999999</v>
-      </c>
-      <c r="S2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="N2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2"/>
     </row>
-    <row r="3" spans="1:30" ht="15">
-      <c r="D3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
+    <row r="3" spans="1:28" ht="15">
+      <c r="D3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>